<commit_message>
Add comperator instruction to isa.txt and truth table
</commit_message>
<xml_diff>
--- a/Temp/Truth Table.xlsx
+++ b/Temp/Truth Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omrani/Documents/Cp-Arch/Computer-Architectures-and-Design/Temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473073AA-026F-4770-9486-03B314464FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33BACAD-D24C-AB4B-A6DB-39C7BB9A6EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="2196" windowWidth="22716" windowHeight="10164" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
+    <workbookView xWindow="20" yWindow="2200" windowWidth="22720" windowHeight="10160" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -57,9 +55,6 @@
     <t>baw</t>
   </si>
   <si>
-    <t>mem2Reg</t>
-  </si>
-  <si>
     <t>Load</t>
   </si>
   <si>
@@ -97,6 +92,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>comp</t>
   </si>
 </sst>
 </file>
@@ -451,57 +449,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEA70A2-8965-4DC9-A193-22A2BB7A08C5}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +545,11 @@
       <c r="N2" s="1">
         <v>1</v>
       </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -588,8 +592,11 @@
       <c r="N3" s="1">
         <v>0</v>
       </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -612,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -630,10 +637,13 @@
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,8 +686,11 @@
       <c r="N5" s="1">
         <v>0</v>
       </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,8 +733,11 @@
       <c r="N6" s="1">
         <v>0</v>
       </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -764,8 +780,11 @@
       <c r="N7" s="1">
         <v>0</v>
       </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -808,48 +827,7 @@
       <c r="N8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
+      <c r="O8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rearranged Files And Truth Table Edited
</commit_message>
<xml_diff>
--- a/Temp/Truth Table.xlsx
+++ b/Temp/Truth Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omrani/Documents/Cp-Arch/Computer-Architectures-and-Design/Temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uni\term4\CA\Computer-Architectures-and-Design\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33BACAD-D24C-AB4B-A6DB-39C7BB9A6EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D562724-B646-412A-86C5-6A7AB4EC27DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="2200" windowWidth="22720" windowHeight="10160" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>branch</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>stri</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>comp</t>
@@ -452,12 +449,12 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -499,10 +496,10 @@
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -596,12 +593,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -618,8 +615,8 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
+      <c r="H4" s="1">
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -636,14 +633,14 @@
       <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>19</v>
+      <c r="N4" s="1">
+        <v>0</v>
       </c>
       <c r="O4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -690,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -737,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -784,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Set truth table for MemToReg
</commit_message>
<xml_diff>
--- a/Temp/Truth Table.xlsx
+++ b/Temp/Truth Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uni\term4\CA\Computer-Architectures-and-Design\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omrani/Documents/Cp-Arch/Computer-Architectures-and-Design/Temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38789AB-DD54-499C-8471-0E9CABF255E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07586BEA-0C2C-334A-9873-EDF24EA8B586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{A286A91F-5E20-4E8B-9C32-FB2F51450B0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>branch</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>memToReg</t>
   </si>
 </sst>
 </file>
@@ -449,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEA70A2-8965-4DC9-A193-22A2BB7A08C5}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -502,7 +505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -596,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -690,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -737,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -784,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -828,6 +831,53 @@
         <v>1</v>
       </c>
       <c r="O8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>